<commit_message>
Bai 32 - Log4j2
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ExcelData.xlsx
+++ b/src/test/resources/testdata/ExcelData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_SeleniumJava_112023\SeleniumTesNGParallel112023\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_SeleniumJava_112023\SeleniumTestNGParallel112023\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051BBEDC-BCF9-4127-9C3F-1FD6645CB361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56ED9F83-9021-4373-8991-2B1B6D2B0C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7896" yWindow="2688" windowWidth="22704" windowHeight="13872" activeTab="1" xr2:uid="{3F9B8930-9BA4-4968-ABB2-543108AD35B3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{3F9B8930-9BA4-4968-ABB2-543108AD35B3}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDataProvider" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -96,9 +94,6 @@
     <t>COUNTRY</t>
   </si>
   <si>
-    <t>Viettel_01</t>
-  </si>
-  <si>
     <t>https://viettel.com.vn</t>
   </si>
   <si>
@@ -117,9 +112,6 @@
     <t>Vietnamese</t>
   </si>
   <si>
-    <t>Viettel_02</t>
-  </si>
-  <si>
     <t>Gold</t>
   </si>
   <si>
@@ -127,6 +119,12 @@
   </si>
   <si>
     <t>HCM</t>
+  </si>
+  <si>
+    <t>Viettel_03</t>
+  </si>
+  <si>
+    <t>Viettel_04</t>
   </si>
 </sst>
 </file>
@@ -137,7 +135,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -146,7 +144,7 @@
       <u/>
       <sz val="14"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -524,13 +522,13 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.765625" customWidth="1"/>
-    <col min="2" max="2" width="11.4609375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.78515625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -546,7 +544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -554,7 +552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -562,7 +560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -570,7 +568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -578,7 +576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -604,25 +602,25 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.23046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.23046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.15234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.3828125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.3828125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.4609375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.84375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.61328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.2109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.2109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.35546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.35546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -657,9 +655,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -668,33 +666,33 @@
         <v>123456</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2">
         <v>12345</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -703,28 +701,28 @@
         <v>123456</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J3">
         <v>12345</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>